<commit_message>
more coding examples, more translated
</commit_message>
<xml_diff>
--- a/codingexamples/6-bivariate-analysis-CramersV.xlsx
+++ b/codingexamples/6-bivariate-analysis-CramersV.xlsx
@@ -24,9 +24,6 @@
     <t>percentages</t>
   </si>
   <si>
-    <t>(a – e)^2 / e</t>
-  </si>
-  <si>
     <t>good</t>
   </si>
   <si>
@@ -45,15 +42,9 @@
     <t>total</t>
   </si>
   <si>
-    <t>observations (a)</t>
-  </si>
-  <si>
     <t>expected (e)</t>
   </si>
   <si>
-    <t>differences (a – e)</t>
-  </si>
-  <si>
     <t>chi-square</t>
   </si>
   <si>
@@ -69,13 +60,22 @@
     <t>=min(#rows,#cols)</t>
   </si>
   <si>
-    <t>=sum( (a-e)^2 / e )</t>
-  </si>
-  <si>
     <t>=sqrt( chi-square / ((k-1)*n) )</t>
   </si>
   <si>
     <t>Cramér's V</t>
+  </si>
+  <si>
+    <t>observed (o)</t>
+  </si>
+  <si>
+    <t>differences (o – e)</t>
+  </si>
+  <si>
+    <t>(o – e)^2 / e</t>
+  </si>
+  <si>
+    <t>=sum( (o-e)^2 / e )</t>
   </si>
 </sst>
 </file>
@@ -217,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -237,6 +237,131 @@
       </top>
       <bottom style="thin">
         <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -260,21 +385,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -282,6 +399,46 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Accent" xfId="1"/>
@@ -581,12 +738,12 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.25" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.25" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="7" customWidth="1"/>
     <col min="5" max="5" width="2.625" customWidth="1"/>
     <col min="6" max="8" width="8.375" customWidth="1"/>
@@ -596,676 +753,676 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="8"/>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="J1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>9</v>
+      </c>
+      <c r="C3" s="8">
         <v>8</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="J1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>8</v>
-      </c>
-      <c r="D3">
+      <c r="D3" s="16">
         <f>SUM(B3:C3)</f>
         <v>17</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="23">
         <f>B3/B$7</f>
         <v>0.40909090909090912</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="24">
         <f>C3/C$7</f>
         <v>0.29629629629629628</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="24">
         <f>D3/D$7</f>
         <v>0.34693877551020408</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="3">
         <f t="shared" ref="J3:L7" si="0">B3/$D3</f>
         <v>0.52941176470588236</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="3">
         <f t="shared" si="0"/>
         <v>0.47058823529411764</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="10">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="17">
         <f>SUM(B4:C4)</f>
         <v>18</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="19">
         <f t="shared" ref="F4:H6" si="1">B4/B$7</f>
         <v>0.36363636363636365</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="20">
         <f t="shared" si="1"/>
         <v>0.37037037037037035</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="20">
         <f t="shared" si="1"/>
         <v>0.36734693877551022</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="3">
         <f t="shared" si="0"/>
         <v>0.44444444444444442</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="3">
         <f t="shared" si="0"/>
         <v>0.55555555555555558</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="10">
         <v>5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="17">
         <f>SUM(B5:C5)</f>
         <v>10</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="19">
         <f t="shared" si="1"/>
         <v>0.22727272727272727</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="20">
         <f t="shared" si="1"/>
         <v>0.18518518518518517</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="20">
         <f t="shared" si="1"/>
         <v>0.20408163265306123</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="3">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="3">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
+      <c r="A6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11">
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="12">
         <v>4</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="18">
         <f>SUM(B6:C6)</f>
         <v>4</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="22">
         <f t="shared" si="1"/>
         <v>0.14814814814814814</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="22">
         <f t="shared" si="1"/>
         <v>8.1632653061224483E-2</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="B7">
+      <c r="B7" s="11">
         <f>SUM(B3:B6)</f>
         <v>22</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="12">
         <f>SUM(C3:C6)</f>
         <v>27</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="18">
         <f>SUM(B7:C7)</f>
         <v>49</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="21">
         <f t="shared" ref="F7" si="2">B7/B$7</f>
         <v>1</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="22">
         <f t="shared" ref="G7" si="3">C7/C$7</f>
         <v>1</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="22">
         <f t="shared" ref="H7" si="4">D7/D$7</f>
         <v>1</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="3">
         <f t="shared" si="0"/>
         <v>0.44897959183673469</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="3">
         <f t="shared" si="0"/>
         <v>0.55102040816326525</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="F9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="J9" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="B10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="F9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="J9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="B10" t="s">
+      <c r="D10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="F10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2">
-        <f>$D3*B$7/$D$7</f>
+      <c r="A11" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="27">
+        <f t="shared" ref="B11:C14" si="5">$D3*B$7/$D$7</f>
         <v>7.6326530612244898</v>
       </c>
-      <c r="C11" s="2">
-        <f>$D3*C$7/$D$7</f>
+      <c r="C11" s="28">
+        <f t="shared" si="5"/>
         <v>9.3673469387755102</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="8">
         <f>SUM(B11:C11)</f>
         <v>17</v>
       </c>
-      <c r="F11" s="3">
-        <f t="shared" ref="F11:H15" si="5">B11/B$15</f>
+      <c r="F11" s="23">
+        <f t="shared" ref="F11:H15" si="6">B11/B$15</f>
         <v>0.34693877551020408</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="24">
+        <f t="shared" si="6"/>
+        <v>0.34693877551020408</v>
+      </c>
+      <c r="H11" s="24">
+        <f t="shared" si="6"/>
+        <v>0.34693877551020408</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" ref="J11:J15" si="7">B11/$D11</f>
+        <v>0.44897959183673469</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" ref="K11:K15" si="8">C11/$D11</f>
+        <v>0.55102040816326525</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" ref="L11:L15" si="9">D11/$D11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="25">
         <f t="shared" si="5"/>
-        <v>0.34693877551020408</v>
-      </c>
-      <c r="H11" s="3">
+        <v>8.0816326530612237</v>
+      </c>
+      <c r="C12" s="26">
         <f t="shared" si="5"/>
-        <v>0.34693877551020408</v>
-      </c>
-      <c r="J11" s="5">
-        <f t="shared" ref="J11:J15" si="6">B11/$D11</f>
-        <v>0.44897959183673469</v>
-      </c>
-      <c r="K11" s="5">
-        <f t="shared" ref="K11:K15" si="7">C11/$D11</f>
-        <v>0.55102040816326525</v>
-      </c>
-      <c r="L11" s="5">
-        <f t="shared" ref="L11:L15" si="8">D11/$D11</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2">
-        <f>$D4*B$7/$D$7</f>
-        <v>8.0816326530612237</v>
-      </c>
-      <c r="C12" s="2">
-        <f>$D4*C$7/$D$7</f>
         <v>9.9183673469387763</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="10">
         <f>SUM(B12:C12)</f>
         <v>18</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="19">
+        <f t="shared" si="6"/>
+        <v>0.36734693877551017</v>
+      </c>
+      <c r="G12" s="20">
+        <f t="shared" si="6"/>
+        <v>0.36734693877551022</v>
+      </c>
+      <c r="H12" s="20">
+        <f t="shared" si="6"/>
+        <v>0.36734693877551022</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="7"/>
+        <v>0.44897959183673464</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="8"/>
+        <v>0.55102040816326536</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="25">
         <f t="shared" si="5"/>
-        <v>0.36734693877551017</v>
-      </c>
-      <c r="G12" s="3">
+        <v>4.4897959183673466</v>
+      </c>
+      <c r="C13" s="26">
         <f t="shared" si="5"/>
-        <v>0.36734693877551022</v>
-      </c>
-      <c r="H12" s="3">
-        <f t="shared" si="5"/>
-        <v>0.36734693877551022</v>
-      </c>
-      <c r="J12" s="5">
-        <f t="shared" si="6"/>
-        <v>0.44897959183673464</v>
-      </c>
-      <c r="K12" s="5">
-        <f t="shared" si="7"/>
-        <v>0.55102040816326536</v>
-      </c>
-      <c r="L12" s="5">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="2">
-        <f>$D5*B$7/$D$7</f>
-        <v>4.4897959183673466</v>
-      </c>
-      <c r="C13" s="2">
-        <f>$D5*C$7/$D$7</f>
         <v>5.5102040816326534</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="10">
         <f>SUM(B13:C13)</f>
         <v>10</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="19">
+        <f t="shared" si="6"/>
+        <v>0.2040816326530612</v>
+      </c>
+      <c r="G13" s="20">
+        <f t="shared" si="6"/>
+        <v>0.20408163265306123</v>
+      </c>
+      <c r="H13" s="20">
+        <f t="shared" si="6"/>
+        <v>0.20408163265306123</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="7"/>
+        <v>0.44897959183673464</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="8"/>
+        <v>0.55102040816326536</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="29">
         <f t="shared" si="5"/>
-        <v>0.2040816326530612</v>
-      </c>
-      <c r="G13" s="3">
+        <v>1.7959183673469388</v>
+      </c>
+      <c r="C14" s="30">
         <f t="shared" si="5"/>
-        <v>0.20408163265306123</v>
-      </c>
-      <c r="H13" s="3">
-        <f t="shared" si="5"/>
-        <v>0.20408163265306123</v>
-      </c>
-      <c r="J13" s="5">
-        <f t="shared" si="6"/>
-        <v>0.44897959183673464</v>
-      </c>
-      <c r="K13" s="5">
-        <f t="shared" si="7"/>
-        <v>0.55102040816326536</v>
-      </c>
-      <c r="L13" s="5">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="2">
-        <f>$D6*B$7/$D$7</f>
-        <v>1.7959183673469388</v>
-      </c>
-      <c r="C14" s="2">
-        <f>$D6*C$7/$D$7</f>
         <v>2.204081632653061</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="12">
         <f>SUM(B14:C14)</f>
         <v>4</v>
       </c>
-      <c r="F14" s="3">
-        <f t="shared" si="5"/>
+      <c r="F14" s="21">
+        <f t="shared" si="6"/>
         <v>8.1632653061224483E-2</v>
       </c>
-      <c r="G14" s="3">
-        <f t="shared" si="5"/>
+      <c r="G14" s="22">
+        <f t="shared" si="6"/>
         <v>8.1632653061224483E-2</v>
       </c>
-      <c r="H14" s="3">
-        <f t="shared" si="5"/>
+      <c r="H14" s="22">
+        <f t="shared" si="6"/>
         <v>8.1632653061224483E-2</v>
       </c>
-      <c r="J14" s="5">
-        <f t="shared" si="6"/>
+      <c r="J14" s="3">
+        <f t="shared" si="7"/>
         <v>0.44897959183673469</v>
       </c>
-      <c r="K14" s="5">
-        <f t="shared" si="7"/>
+      <c r="K14" s="3">
+        <f t="shared" si="8"/>
         <v>0.55102040816326525</v>
       </c>
-      <c r="L14" s="5">
-        <f t="shared" si="8"/>
+      <c r="L14" s="3">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="B15">
+      <c r="B15" s="11">
         <f>SUM(B11:B14)</f>
         <v>22</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="12">
         <f>SUM(C11:C14)</f>
         <v>27</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="12">
         <f>SUM(B15:C15)</f>
         <v>49</v>
       </c>
-      <c r="F15" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="G15" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H15" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="J15" s="5">
+      <c r="F15" s="21">
         <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G15" s="22">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H15" s="22">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="7"/>
         <v>0.44897959183673469</v>
       </c>
-      <c r="K15" s="5">
-        <f t="shared" si="7"/>
+      <c r="K15" s="3">
+        <f t="shared" si="8"/>
         <v>0.55102040816326525</v>
       </c>
-      <c r="L15" s="5">
-        <f t="shared" si="8"/>
+      <c r="L15" s="3">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="B17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B17" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
+      <c r="B18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="27">
+        <f t="shared" ref="B19:C22" si="10">B3-B11</f>
+        <v>1.3673469387755102</v>
+      </c>
+      <c r="C19" s="28">
+        <f t="shared" si="10"/>
+        <v>-1.3673469387755102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="2">
-        <f t="shared" ref="B19:C22" si="9">B3-B11</f>
-        <v>1.3673469387755102</v>
-      </c>
-      <c r="C19" s="2">
-        <f t="shared" si="9"/>
-        <v>-1.3673469387755102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="9" t="s">
+      <c r="B20" s="25">
+        <f t="shared" si="10"/>
+        <v>-8.1632653061223692E-2</v>
+      </c>
+      <c r="C20" s="26">
+        <f t="shared" si="10"/>
+        <v>8.1632653061223692E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="2">
-        <f t="shared" si="9"/>
-        <v>-8.1632653061223692E-2</v>
-      </c>
-      <c r="C20" s="2">
-        <f t="shared" si="9"/>
-        <v>8.1632653061223692E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="9" t="s">
+      <c r="B21" s="25">
+        <f t="shared" si="10"/>
+        <v>0.51020408163265341</v>
+      </c>
+      <c r="C21" s="26">
+        <f t="shared" si="10"/>
+        <v>-0.51020408163265341</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="2">
-        <f t="shared" si="9"/>
-        <v>0.51020408163265341</v>
-      </c>
-      <c r="C21" s="2">
-        <f t="shared" si="9"/>
-        <v>-0.51020408163265341</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="2">
-        <f t="shared" si="9"/>
+      <c r="B22" s="29">
+        <f t="shared" si="10"/>
         <v>-1.7959183673469388</v>
       </c>
-      <c r="C22" s="2">
-        <f t="shared" si="9"/>
+      <c r="C22" s="30">
+        <f t="shared" si="10"/>
         <v>1.795918367346939</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="B24" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>12</v>
+      <c r="B25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="7">
+        <f t="shared" ref="B26:C29" si="11">(B19*B19)/B11</f>
+        <v>0.24495252646513149</v>
+      </c>
+      <c r="C26" s="8">
+        <f t="shared" si="11"/>
+        <v>0.19959094749010714</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B26">
-        <f t="shared" ref="B26:C29" si="10">(B19*B19)/B11</f>
-        <v>0.24495252646513149</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="10"/>
-        <v>0.19959094749010714</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="9" t="s">
+      <c r="B27" s="9">
+        <f t="shared" si="11"/>
+        <v>8.2457225314366573E-4</v>
+      </c>
+      <c r="C27" s="10">
+        <f t="shared" si="11"/>
+        <v>6.7187368774669046E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B27">
-        <f t="shared" si="10"/>
-        <v>8.2457225314366573E-4</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="10"/>
-        <v>6.7187368774669046E-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="9" t="s">
+      <c r="B28" s="9">
+        <f t="shared" si="11"/>
+        <v>5.7977736549165201E-2</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" si="11"/>
+        <v>4.7241118669690156E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B28">
-        <f t="shared" si="10"/>
-        <v>5.7977736549165201E-2</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="10"/>
-        <v>4.7241118669690156E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29">
-        <f t="shared" si="10"/>
+      <c r="B29" s="11">
+        <f t="shared" si="11"/>
         <v>1.7959183673469388</v>
       </c>
-      <c r="C29">
-        <f t="shared" si="10"/>
+      <c r="C29" s="12">
+        <f t="shared" si="11"/>
         <v>1.463340891912321</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31">
+      <c r="A31" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="34">
         <f>SUM(B26:C29)</f>
         <v>3.810518034374244</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
+      <c r="C31" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="9" t="s">
-        <v>14</v>
+      <c r="A32" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B32">
         <f>MIN(COUNT(B7:C7),COUNT(D3:D6))</f>
         <v>2</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>15</v>
+      <c r="C32" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="9" t="s">
-        <v>13</v>
+      <c r="A33" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="B33">
         <f>D7</f>
         <v>49</v>
       </c>
-      <c r="C33" s="10"/>
+      <c r="C33" s="6"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34">
+      <c r="A34" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="34">
         <f>SQRT(B31/((B32-1)*B33))</f>
         <v>0.27886497480125205</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>17</v>
+      <c r="C34" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>